<commit_message>
output folder structure update
</commit_message>
<xml_diff>
--- a/input/calibration/tagem-arge-toprak-analiz-sonuclari.xlsx
+++ b/input/calibration/tagem-arge-toprak-analiz-sonuclari.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurg\Documents\GitHub\oceanview\input\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurgudelek\Documents\GitHub\Libs\input\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED358B8-92BB-4448-ADE5-597FCB9C7CF5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA70158-8569-4A46-BB06-54014470D64C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adana" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="32">
   <si>
     <t>SIRA NO</t>
   </si>
@@ -53,231 +53,6 @@
   </si>
   <si>
     <t>NİĞDE-BOR</t>
-  </si>
-  <si>
-    <t>4,88</t>
-  </si>
-  <si>
-    <t>1,76</t>
-  </si>
-  <si>
-    <t>12,68</t>
-  </si>
-  <si>
-    <t>4,2</t>
-  </si>
-  <si>
-    <t>1,69</t>
-  </si>
-  <si>
-    <t>2,91</t>
-  </si>
-  <si>
-    <t>7,86</t>
-  </si>
-  <si>
-    <t>21,5</t>
-  </si>
-  <si>
-    <t>9,42</t>
-  </si>
-  <si>
-    <t>5,69</t>
-  </si>
-  <si>
-    <t>2,98</t>
-  </si>
-  <si>
-    <t>4,61</t>
-  </si>
-  <si>
-    <t>5,76</t>
-  </si>
-  <si>
-    <t>13,02</t>
-  </si>
-  <si>
-    <t>20,48</t>
-  </si>
-  <si>
-    <t>3,93</t>
-  </si>
-  <si>
-    <t>1,48</t>
-  </si>
-  <si>
-    <t>1,82</t>
-  </si>
-  <si>
-    <t>2,71</t>
-  </si>
-  <si>
-    <t>6,78</t>
-  </si>
-  <si>
-    <t>3,66</t>
-  </si>
-  <si>
-    <t>2,5</t>
-  </si>
-  <si>
-    <t>1,28</t>
-  </si>
-  <si>
-    <t>47,3</t>
-  </si>
-  <si>
-    <t>12,79</t>
-  </si>
-  <si>
-    <t>35,42</t>
-  </si>
-  <si>
-    <t>32,04</t>
-  </si>
-  <si>
-    <t>8,46</t>
-  </si>
-  <si>
-    <t>55,84</t>
-  </si>
-  <si>
-    <t>112,61</t>
-  </si>
-  <si>
-    <t>37,05</t>
-  </si>
-  <si>
-    <t>65,05</t>
-  </si>
-  <si>
-    <t>39,2</t>
-  </si>
-  <si>
-    <t>81,66</t>
-  </si>
-  <si>
-    <t>37,76</t>
-  </si>
-  <si>
-    <t>32,48</t>
-  </si>
-  <si>
-    <t>166,88</t>
-  </si>
-  <si>
-    <t>203,81</t>
-  </si>
-  <si>
-    <t>34,05</t>
-  </si>
-  <si>
-    <t>17,67</t>
-  </si>
-  <si>
-    <t>71,67</t>
-  </si>
-  <si>
-    <t>73,94</t>
-  </si>
-  <si>
-    <t>52,73</t>
-  </si>
-  <si>
-    <t>57,28</t>
-  </si>
-  <si>
-    <t>69,11</t>
-  </si>
-  <si>
-    <t>16,02</t>
-  </si>
-  <si>
-    <t>0,25</t>
-  </si>
-  <si>
-    <t>0,73</t>
-  </si>
-  <si>
-    <t>1,04</t>
-  </si>
-  <si>
-    <t>0,89</t>
-  </si>
-  <si>
-    <t>1,01</t>
-  </si>
-  <si>
-    <t>0,85</t>
-  </si>
-  <si>
-    <t>0,62</t>
-  </si>
-  <si>
-    <t>0,59</t>
-  </si>
-  <si>
-    <t>1,55</t>
-  </si>
-  <si>
-    <t>0,17</t>
-  </si>
-  <si>
-    <t>1,25</t>
-  </si>
-  <si>
-    <t>1,6</t>
-  </si>
-  <si>
-    <t>1,54</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>0,79</t>
-  </si>
-  <si>
-    <t>1,4</t>
-  </si>
-  <si>
-    <t>0,83</t>
-  </si>
-  <si>
-    <t>1,24</t>
-  </si>
-  <si>
-    <t>1,44</t>
-  </si>
-  <si>
-    <t>0,51</t>
-  </si>
-  <si>
-    <t>0,19</t>
-  </si>
-  <si>
-    <t>0,01</t>
-  </si>
-  <si>
-    <t>0,04</t>
-  </si>
-  <si>
-    <t>0,05</t>
-  </si>
-  <si>
-    <t>0,03</t>
-  </si>
-  <si>
-    <t>0,08</t>
-  </si>
-  <si>
-    <t>0,06</t>
-  </si>
-  <si>
-    <t>0,07</t>
-  </si>
-  <si>
-    <t>10,05</t>
   </si>
   <si>
     <t>C 1 @ 279.482</t>
@@ -350,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,11 +679,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="5"/>
     <col min="3" max="3" width="9.140625" style="1"/>
@@ -927,7 +702,7 @@
     <col min="26" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="8" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -963,7 +738,7 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="4" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -977,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
@@ -986,70 +761,70 @@
         <v>6</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="W2" s="19" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="Y2" s="19" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="AA2" s="19" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="AB2" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -1093,7 +868,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -1137,7 +912,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1181,7 +956,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1225,7 +1000,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1269,7 +1044,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1313,7 +1088,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1357,7 +1132,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1401,7 +1176,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1445,7 +1220,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1489,7 +1264,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -1533,7 +1308,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1577,7 +1352,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -1621,7 +1396,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -1665,7 +1440,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -1709,7 +1484,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -1753,7 +1528,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -1797,7 +1572,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -1841,7 +1616,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -1885,7 +1660,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -1929,7 +1704,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -1973,7 +1748,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -2017,7 +1792,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -2061,7 +1836,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -2105,7 +1880,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -2149,7 +1924,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -2193,7 +1968,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -2237,7 +2012,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -2281,7 +2056,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -2325,7 +2100,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -2369,7 +2144,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -2413,7 +2188,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -2457,7 +2232,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -2501,7 +2276,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -2545,7 +2320,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -2589,7 +2364,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -2633,7 +2408,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -2677,7 +2452,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -2721,7 +2496,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -2765,7 +2540,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -2809,7 +2584,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -2853,7 +2628,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -2897,7 +2672,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -2941,7 +2716,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -2985,7 +2760,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -3029,7 +2804,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -3073,7 +2848,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -3117,7 +2892,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -3161,7 +2936,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -3205,7 +2980,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -3263,11 +3038,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P1" sqref="A1:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -3281,7 +3056,7 @@
     <col min="26" max="28" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="8" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -3317,7 +3092,7 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="4" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3106,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
@@ -3340,70 +3115,70 @@
         <v>6</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="W2" s="19" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="Y2" s="19" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="AA2" s="19" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="AB2" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3413,17 +3188,17 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
+      <c r="D3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F3" s="2">
+        <v>47.3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.88</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -3447,7 +3222,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -3457,17 +3232,17 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
+      <c r="D4" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="F4" s="2">
+        <v>12.79</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.76</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -3491,7 +3266,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -3501,17 +3276,17 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
+      <c r="D5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="F5" s="2">
+        <v>35.42</v>
+      </c>
+      <c r="G5" s="2">
+        <v>12.68</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -3535,7 +3310,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3545,17 +3320,17 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
+      <c r="D6" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="F6" s="2">
+        <v>32.04</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.2</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -3579,7 +3354,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3589,17 +3364,17 @@
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>14</v>
+      <c r="D7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="F7" s="2">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.69</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
@@ -3623,7 +3398,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3633,17 +3408,17 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
+      <c r="D8" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F8" s="2">
+        <v>55.84</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2.91</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -3667,7 +3442,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3677,17 +3452,17 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>16</v>
+      <c r="D9" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="F9" s="2">
+        <v>112.61</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7.86</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -3711,7 +3486,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3721,17 +3496,17 @@
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>17</v>
+      <c r="D10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F10" s="2">
+        <v>37.049999999999997</v>
+      </c>
+      <c r="G10" s="2">
+        <v>21.5</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -3755,7 +3530,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3765,17 +3540,17 @@
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>18</v>
+      <c r="D11" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="F11" s="2">
+        <v>65.05</v>
+      </c>
+      <c r="G11" s="2">
+        <v>9.42</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -3799,7 +3574,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3809,17 +3584,17 @@
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
+      <c r="D12" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="F12" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5.69</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
@@ -3843,7 +3618,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3853,17 +3628,17 @@
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>20</v>
+      <c r="D13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="F13" s="2">
+        <v>81.66</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.98</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -3887,7 +3662,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3897,17 +3672,17 @@
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
+      <c r="D14" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F14" s="2">
+        <v>37.76</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4.6100000000000003</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -3931,7 +3706,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3941,17 +3716,17 @@
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>20</v>
+      <c r="D15" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="F15" s="2">
+        <v>32.479999999999997</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.98</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
@@ -3975,7 +3750,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3985,17 +3760,17 @@
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>21</v>
+      <c r="D16" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="F16" s="2">
+        <v>166.88</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4.6100000000000003</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
@@ -4019,7 +3794,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -4029,17 +3804,17 @@
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>22</v>
+      <c r="D17" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="F17" s="2">
+        <v>203.81</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5.76</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
@@ -4063,7 +3838,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -4073,17 +3848,17 @@
       <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>23</v>
+      <c r="D18" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>34.049999999999997</v>
+      </c>
+      <c r="G18" s="2">
+        <v>13.02</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
@@ -4107,7 +3882,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -4117,17 +3892,17 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>24</v>
+      <c r="D19" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="F19" s="2">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="G19" s="2">
+        <v>20.48</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
@@ -4151,7 +3926,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -4161,17 +3936,17 @@
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>25</v>
+      <c r="D20" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F20" s="2">
+        <v>71.67</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3.93</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
@@ -4195,7 +3970,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -4205,17 +3980,17 @@
       <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>26</v>
+      <c r="D21" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>35.42</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.48</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
@@ -4239,7 +4014,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -4249,17 +4024,17 @@
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>27</v>
+      <c r="D22" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="F22" s="2">
+        <v>73.94</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.82</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
@@ -4283,7 +4058,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -4293,17 +4068,17 @@
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>28</v>
+      <c r="D23" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="F23" s="2">
+        <v>52.73</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2.71</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
@@ -4327,7 +4102,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -4337,17 +4112,17 @@
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>29</v>
+      <c r="D24" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="F24" s="2">
+        <v>57.28</v>
+      </c>
+      <c r="G24" s="2">
+        <v>6.78</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
@@ -4371,7 +4146,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -4381,17 +4156,17 @@
       <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>30</v>
+      <c r="D25" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.44</v>
+      </c>
+      <c r="F25" s="2">
+        <v>69.11</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3.66</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
@@ -4415,7 +4190,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -4425,17 +4200,17 @@
       <c r="C26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>31</v>
+      <c r="D26" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="F26" s="2">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2.5</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
@@ -4459,7 +4234,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -4469,17 +4244,17 @@
       <c r="C27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>32</v>
+      <c r="D27" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="F27" s="2">
+        <v>16.02</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1.28</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
@@ -4503,7 +4278,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28">
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -4526,7 +4301,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28">
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -4549,7 +4324,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28">
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -4572,7 +4347,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28">
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -4595,7 +4370,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28">
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -4618,7 +4393,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:28">
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -4641,7 +4416,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:28">
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -4664,7 +4439,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:28">
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -4687,7 +4462,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:28">
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
@@ -4710,7 +4485,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:28">
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -4733,7 +4508,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:28">
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
@@ -4756,7 +4531,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:28">
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
@@ -4779,7 +4554,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:28">
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
@@ -4802,7 +4577,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:28">
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
@@ -4825,7 +4600,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:28">
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
@@ -4848,7 +4623,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:28">
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
@@ -4871,7 +4646,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:28">
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -4894,7 +4669,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:28">
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -4917,7 +4692,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:28">
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -4940,7 +4715,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:28">
       <c r="H47" s="20"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -4963,7 +4738,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:28">
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -4986,7 +4761,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:28">
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -5009,7 +4784,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:28">
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -5032,7 +4807,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:28">
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -5055,7 +4830,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:28">
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -5096,7 +4871,7 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="6"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
@@ -5111,7 +4886,7 @@
     <col min="26" max="28" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="8" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -5147,7 +4922,7 @@
       <c r="AA1" s="22"/>
       <c r="AB1" s="22"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5161,7 +4936,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
@@ -5170,70 +4945,70 @@
         <v>6</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="W2" s="19" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="Y2" s="19" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="AA2" s="19" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="AB2" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -5277,7 +5052,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -5321,7 +5096,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -5365,7 +5140,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -5409,7 +5184,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -5453,7 +5228,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -5497,7 +5272,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -5541,7 +5316,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -5585,7 +5360,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -5629,7 +5404,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -5673,7 +5448,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -5717,7 +5492,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -5761,7 +5536,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -5805,7 +5580,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -5849,7 +5624,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -5893,7 +5668,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -5937,7 +5712,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -5981,7 +5756,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -6025,7 +5800,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -6069,7 +5844,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -6113,7 +5888,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -6157,7 +5932,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -6201,7 +5976,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -6245,7 +6020,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -6289,7 +6064,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -6333,7 +6108,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28">
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -6356,7 +6131,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28">
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -6379,7 +6154,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28">
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -6402,7 +6177,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28">
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -6425,7 +6200,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28">
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -6448,7 +6223,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:28">
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -6471,7 +6246,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:28">
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -6494,7 +6269,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:28">
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -6517,7 +6292,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:28">
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
@@ -6540,7 +6315,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:28">
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -6563,7 +6338,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:28">
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
@@ -6586,7 +6361,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:28">
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
@@ -6609,7 +6384,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:28">
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
@@ -6632,7 +6407,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:28">
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
@@ -6655,7 +6430,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:28">
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
@@ -6678,7 +6453,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:28">
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
@@ -6701,7 +6476,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:28">
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -6724,7 +6499,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:28">
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -6747,7 +6522,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:28">
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -6770,7 +6545,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:28">
       <c r="H47" s="20"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -6793,7 +6568,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:28">
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -6816,7 +6591,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:28">
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -6839,7 +6614,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:28">
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -6862,7 +6637,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:28">
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -6885,7 +6660,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="8:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:28">
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -6922,11 +6697,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="10.140625" style="5" customWidth="1"/>
@@ -6945,7 +6720,7 @@
     <col min="29" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="8" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -6981,7 +6756,7 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6995,7 +6770,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
@@ -7004,70 +6779,70 @@
         <v>6</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="W2" s="19" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="Y2" s="19" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="AA2" s="19" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="AB2" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="14.1" customHeight="1">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -7111,7 +6886,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="14.1" customHeight="1">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -7155,7 +6930,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="14.1" customHeight="1">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -7199,7 +6974,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="14.1" customHeight="1">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -7243,7 +7018,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="14.1" customHeight="1">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -7287,7 +7062,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="14.1" customHeight="1">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -7331,7 +7106,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="14.1" customHeight="1">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -7375,7 +7150,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="14.1" customHeight="1">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -7419,7 +7194,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="14.1" customHeight="1">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -7463,7 +7238,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="14.1" customHeight="1">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -7507,7 +7282,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="14.1" customHeight="1">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -7551,7 +7326,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="14.1" customHeight="1">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -7595,7 +7370,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="14.1" customHeight="1">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -7639,7 +7414,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="14.1" customHeight="1">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -7683,7 +7458,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="14.1" customHeight="1">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -7727,7 +7502,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="14.1" customHeight="1">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -7771,7 +7546,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="14.1" customHeight="1">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -7815,7 +7590,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="14.1" customHeight="1">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -7859,7 +7634,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="14.1" customHeight="1">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -7903,7 +7678,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="14.1" customHeight="1">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -7947,7 +7722,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="14.1" customHeight="1">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -7991,7 +7766,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="14.1" customHeight="1">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -8035,7 +7810,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="14.1" customHeight="1">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -8079,7 +7854,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="14.1" customHeight="1">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -8123,7 +7898,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="14.1" customHeight="1">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -8167,7 +7942,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="14.1" customHeight="1">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -8211,7 +7986,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="14.1" customHeight="1">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -8255,7 +8030,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="14.1" customHeight="1">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -8299,7 +8074,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="14.1" customHeight="1">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -8343,7 +8118,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="14.1" customHeight="1">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -8387,7 +8162,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="14.1" customHeight="1">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -8431,7 +8206,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="14.1" customHeight="1">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -8475,7 +8250,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="14.1" customHeight="1">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -8519,7 +8294,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="14.1" customHeight="1">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -8563,7 +8338,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="14.1" customHeight="1">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -8607,7 +8382,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="14.1" customHeight="1">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -8651,7 +8426,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="14.1" customHeight="1">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -8695,7 +8470,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="14.1" customHeight="1">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -8739,7 +8514,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="14.1" customHeight="1">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -8783,7 +8558,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="14.1" customHeight="1">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -8827,7 +8602,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="14.1" customHeight="1">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -8871,7 +8646,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="14.1" customHeight="1">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -8915,7 +8690,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="14.1" customHeight="1">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -8959,7 +8734,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="14.1" customHeight="1">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -9003,7 +8778,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="14.1" customHeight="1">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -9047,7 +8822,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="14.1" customHeight="1">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -9091,7 +8866,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="14.1" customHeight="1">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -9135,7 +8910,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="14.1" customHeight="1">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -9179,7 +8954,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="14.1" customHeight="1">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -9223,7 +8998,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="14.1" customHeight="1">
       <c r="A52" s="10">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
trying to implement bokeh plot. select event trigger should be triggered!
</commit_message>
<xml_diff>
--- a/input/calibration/tagem-arge-toprak-analiz-sonuclari.xlsx
+++ b/input/calibration/tagem-arge-toprak-analiz-sonuclari.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurgudelek\Documents\GitHub\Libs\input\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurg\Documents\GitHub\oceanview\input\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA70158-8569-4A46-BB06-54014470D64C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCEAE31-C014-46E6-AE3A-C31322B86DD8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,7 +683,7 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="5"/>
     <col min="3" max="3" width="9.140625" style="1"/>
@@ -702,7 +702,7 @@
     <col min="26" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1">
+    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -738,7 +738,7 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28" s="4" customFormat="1">
+    <row r="2" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -824,7 +824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="3" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1000,7 +1000,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="7" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1044,7 +1044,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="8" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1088,7 +1088,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="9" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="10" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="11" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1220,7 +1220,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="12" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="13" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="14" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1352,7 +1352,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="15" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="16" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -1440,7 +1440,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="17" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -1484,7 +1484,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="18" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -1528,7 +1528,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="19" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="20" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="21" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="22" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="23" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -1748,7 +1748,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="24" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -1792,7 +1792,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="25" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="26" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -1880,7 +1880,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="27" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="28" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -1968,7 +1968,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="29" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="30" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="31" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="32" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -2144,7 +2144,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="33" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -2188,7 +2188,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="34" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="35" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="36" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -2320,7 +2320,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="37" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="38" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="39" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -2452,7 +2452,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="40" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="41" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="42" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="43" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -2628,7 +2628,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="44" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -2672,7 +2672,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="45" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -2716,7 +2716,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="46" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="47" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="48" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="49" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="50" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -2936,7 +2936,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="51" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -2980,7 +2980,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1">
+    <row r="52" spans="1:28" s="9" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -3042,7 +3042,7 @@
       <selection activeCell="D3" sqref="D3:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -3056,7 +3056,7 @@
     <col min="26" max="28" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1">
+    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -3092,7 +3092,7 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28" s="4" customFormat="1">
+    <row r="2" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -3266,7 +3266,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3354,7 +3354,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3442,7 +3442,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3530,7 +3530,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3618,7 +3618,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3662,7 +3662,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3750,7 +3750,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3926,7 +3926,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3970,7 +3970,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -4058,7 +4058,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -4102,7 +4102,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -4146,7 +4146,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -4190,7 +4190,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -4234,7 +4234,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -4278,7 +4278,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -4301,7 +4301,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -4324,7 +4324,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -4347,7 +4347,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -4370,7 +4370,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -4393,7 +4393,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="8:28">
+    <row r="33" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -4416,7 +4416,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="8:28">
+    <row r="34" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -4439,7 +4439,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="8:28">
+    <row r="35" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -4462,7 +4462,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="8:28">
+    <row r="36" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
@@ -4485,7 +4485,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="8:28">
+    <row r="37" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -4508,7 +4508,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="8:28">
+    <row r="38" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
@@ -4531,7 +4531,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="8:28">
+    <row r="39" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
@@ -4554,7 +4554,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="8:28">
+    <row r="40" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
@@ -4577,7 +4577,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="8:28">
+    <row r="41" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
@@ -4600,7 +4600,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="8:28">
+    <row r="42" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
@@ -4623,7 +4623,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="8:28">
+    <row r="43" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
@@ -4646,7 +4646,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="8:28">
+    <row r="44" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -4669,7 +4669,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="8:28">
+    <row r="45" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -4692,7 +4692,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="8:28">
+    <row r="46" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -4715,7 +4715,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="8:28">
+    <row r="47" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H47" s="20"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -4738,7 +4738,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="8:28">
+    <row r="48" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -4761,7 +4761,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="8:28">
+    <row r="49" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -4784,7 +4784,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="8:28">
+    <row r="50" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -4807,7 +4807,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="8:28">
+    <row r="51" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -4830,7 +4830,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="8:28">
+    <row r="52" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -4871,7 +4871,7 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="6"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
@@ -4886,7 +4886,7 @@
     <col min="26" max="28" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1">
+    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -4922,7 +4922,7 @@
       <c r="AA1" s="22"/>
       <c r="AB1" s="22"/>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -5052,7 +5052,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -5096,7 +5096,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -5140,7 +5140,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -5184,7 +5184,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -5228,7 +5228,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -5272,7 +5272,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -5316,7 +5316,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -5404,7 +5404,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -5448,7 +5448,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -5536,7 +5536,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -5580,7 +5580,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -5668,7 +5668,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -5712,7 +5712,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -5756,7 +5756,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -5800,7 +5800,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -5844,7 +5844,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -5888,7 +5888,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -5932,7 +5932,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -5976,7 +5976,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -6020,7 +6020,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -6064,7 +6064,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -6108,7 +6108,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -6131,7 +6131,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -6154,7 +6154,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -6177,7 +6177,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -6200,7 +6200,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -6223,7 +6223,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="8:28">
+    <row r="33" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -6246,7 +6246,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="8:28">
+    <row r="34" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -6269,7 +6269,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="8:28">
+    <row r="35" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -6292,7 +6292,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="8:28">
+    <row r="36" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
@@ -6315,7 +6315,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="8:28">
+    <row r="37" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -6338,7 +6338,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="8:28">
+    <row r="38" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
@@ -6361,7 +6361,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="8:28">
+    <row r="39" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
@@ -6384,7 +6384,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="8:28">
+    <row r="40" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
@@ -6407,7 +6407,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="8:28">
+    <row r="41" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
@@ -6430,7 +6430,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="8:28">
+    <row r="42" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
@@ -6453,7 +6453,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="8:28">
+    <row r="43" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
@@ -6476,7 +6476,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="8:28">
+    <row r="44" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -6499,7 +6499,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="8:28">
+    <row r="45" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -6522,7 +6522,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="8:28">
+    <row r="46" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -6545,7 +6545,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="8:28">
+    <row r="47" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H47" s="20"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -6568,7 +6568,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="8:28">
+    <row r="48" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -6591,7 +6591,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="8:28">
+    <row r="49" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -6614,7 +6614,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="8:28">
+    <row r="50" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -6637,7 +6637,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="8:28">
+    <row r="51" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -6660,7 +6660,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="8:28">
+    <row r="52" spans="8:28" x14ac:dyDescent="0.25">
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -6701,7 +6701,7 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="10.140625" style="5" customWidth="1"/>
@@ -6720,7 +6720,7 @@
     <col min="29" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1">
+    <row r="1" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
@@ -6756,7 +6756,7 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="14.1" customHeight="1">
+    <row r="3" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -6886,7 +6886,7 @@
       <c r="AA3" s="20"/>
       <c r="AB3" s="20"/>
     </row>
-    <row r="4" spans="1:28" ht="14.1" customHeight="1">
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -6930,7 +6930,7 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
     </row>
-    <row r="5" spans="1:28" ht="14.1" customHeight="1">
+    <row r="5" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -6974,7 +6974,7 @@
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
     </row>
-    <row r="6" spans="1:28" ht="14.1" customHeight="1">
+    <row r="6" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -7018,7 +7018,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
     </row>
-    <row r="7" spans="1:28" ht="14.1" customHeight="1">
+    <row r="7" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -7062,7 +7062,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
     </row>
-    <row r="8" spans="1:28" ht="14.1" customHeight="1">
+    <row r="8" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -7106,7 +7106,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:28" ht="14.1" customHeight="1">
+    <row r="9" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -7150,7 +7150,7 @@
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
     </row>
-    <row r="10" spans="1:28" ht="14.1" customHeight="1">
+    <row r="10" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -7194,7 +7194,7 @@
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
     </row>
-    <row r="11" spans="1:28" ht="14.1" customHeight="1">
+    <row r="11" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -7238,7 +7238,7 @@
       <c r="AA11" s="20"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" spans="1:28" ht="14.1" customHeight="1">
+    <row r="12" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -7282,7 +7282,7 @@
       <c r="AA12" s="20"/>
       <c r="AB12" s="20"/>
     </row>
-    <row r="13" spans="1:28" ht="14.1" customHeight="1">
+    <row r="13" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -7326,7 +7326,7 @@
       <c r="AA13" s="20"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" spans="1:28" ht="14.1" customHeight="1">
+    <row r="14" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -7370,7 +7370,7 @@
       <c r="AA14" s="20"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" ht="14.1" customHeight="1">
+    <row r="15" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -7414,7 +7414,7 @@
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" ht="14.1" customHeight="1">
+    <row r="16" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -7458,7 +7458,7 @@
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
     </row>
-    <row r="17" spans="1:28" ht="14.1" customHeight="1">
+    <row r="17" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -7502,7 +7502,7 @@
       <c r="AA17" s="20"/>
       <c r="AB17" s="20"/>
     </row>
-    <row r="18" spans="1:28" ht="14.1" customHeight="1">
+    <row r="18" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -7546,7 +7546,7 @@
       <c r="AA18" s="20"/>
       <c r="AB18" s="20"/>
     </row>
-    <row r="19" spans="1:28" ht="14.1" customHeight="1">
+    <row r="19" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -7590,7 +7590,7 @@
       <c r="AA19" s="20"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" spans="1:28" ht="14.1" customHeight="1">
+    <row r="20" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -7634,7 +7634,7 @@
       <c r="AA20" s="20"/>
       <c r="AB20" s="20"/>
     </row>
-    <row r="21" spans="1:28" ht="14.1" customHeight="1">
+    <row r="21" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -7678,7 +7678,7 @@
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
     </row>
-    <row r="22" spans="1:28" ht="14.1" customHeight="1">
+    <row r="22" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -7722,7 +7722,7 @@
       <c r="AA22" s="20"/>
       <c r="AB22" s="20"/>
     </row>
-    <row r="23" spans="1:28" ht="14.1" customHeight="1">
+    <row r="23" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -7766,7 +7766,7 @@
       <c r="AA23" s="20"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" spans="1:28" ht="14.1" customHeight="1">
+    <row r="24" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -7810,7 +7810,7 @@
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" spans="1:28" ht="14.1" customHeight="1">
+    <row r="25" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -7854,7 +7854,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" spans="1:28" ht="14.1" customHeight="1">
+    <row r="26" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -7898,7 +7898,7 @@
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" spans="1:28" ht="14.1" customHeight="1">
+    <row r="27" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -7942,7 +7942,7 @@
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
     </row>
-    <row r="28" spans="1:28" ht="14.1" customHeight="1">
+    <row r="28" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -7986,7 +7986,7 @@
       <c r="AA28" s="20"/>
       <c r="AB28" s="20"/>
     </row>
-    <row r="29" spans="1:28" ht="14.1" customHeight="1">
+    <row r="29" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -8030,7 +8030,7 @@
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="1:28" ht="14.1" customHeight="1">
+    <row r="30" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -8074,7 +8074,7 @@
       <c r="AA30" s="20"/>
       <c r="AB30" s="20"/>
     </row>
-    <row r="31" spans="1:28" ht="14.1" customHeight="1">
+    <row r="31" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -8118,7 +8118,7 @@
       <c r="AA31" s="20"/>
       <c r="AB31" s="20"/>
     </row>
-    <row r="32" spans="1:28" ht="14.1" customHeight="1">
+    <row r="32" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -8162,7 +8162,7 @@
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
     </row>
-    <row r="33" spans="1:28" ht="14.1" customHeight="1">
+    <row r="33" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -8206,7 +8206,7 @@
       <c r="AA33" s="20"/>
       <c r="AB33" s="20"/>
     </row>
-    <row r="34" spans="1:28" ht="14.1" customHeight="1">
+    <row r="34" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -8250,7 +8250,7 @@
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
     </row>
-    <row r="35" spans="1:28" ht="14.1" customHeight="1">
+    <row r="35" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -8294,7 +8294,7 @@
       <c r="AA35" s="20"/>
       <c r="AB35" s="20"/>
     </row>
-    <row r="36" spans="1:28" ht="14.1" customHeight="1">
+    <row r="36" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -8338,7 +8338,7 @@
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="1:28" ht="14.1" customHeight="1">
+    <row r="37" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -8382,7 +8382,7 @@
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
     </row>
-    <row r="38" spans="1:28" ht="14.1" customHeight="1">
+    <row r="38" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -8426,7 +8426,7 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
     </row>
-    <row r="39" spans="1:28" ht="14.1" customHeight="1">
+    <row r="39" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -8470,7 +8470,7 @@
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
     </row>
-    <row r="40" spans="1:28" ht="14.1" customHeight="1">
+    <row r="40" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -8514,7 +8514,7 @@
       <c r="AA40" s="20"/>
       <c r="AB40" s="20"/>
     </row>
-    <row r="41" spans="1:28" ht="14.1" customHeight="1">
+    <row r="41" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -8558,7 +8558,7 @@
       <c r="AA41" s="20"/>
       <c r="AB41" s="20"/>
     </row>
-    <row r="42" spans="1:28" ht="14.1" customHeight="1">
+    <row r="42" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -8602,7 +8602,7 @@
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
     </row>
-    <row r="43" spans="1:28" ht="14.1" customHeight="1">
+    <row r="43" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -8646,7 +8646,7 @@
       <c r="AA43" s="20"/>
       <c r="AB43" s="20"/>
     </row>
-    <row r="44" spans="1:28" ht="14.1" customHeight="1">
+    <row r="44" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -8690,7 +8690,7 @@
       <c r="AA44" s="20"/>
       <c r="AB44" s="20"/>
     </row>
-    <row r="45" spans="1:28" ht="14.1" customHeight="1">
+    <row r="45" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -8734,7 +8734,7 @@
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="1:28" ht="14.1" customHeight="1">
+    <row r="46" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -8778,7 +8778,7 @@
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="1:28" ht="14.1" customHeight="1">
+    <row r="47" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -8822,7 +8822,7 @@
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="1:28" ht="14.1" customHeight="1">
+    <row r="48" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -8866,7 +8866,7 @@
       <c r="AA48" s="20"/>
       <c r="AB48" s="20"/>
     </row>
-    <row r="49" spans="1:28" ht="14.1" customHeight="1">
+    <row r="49" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -8910,7 +8910,7 @@
       <c r="AA49" s="20"/>
       <c r="AB49" s="20"/>
     </row>
-    <row r="50" spans="1:28" ht="14.1" customHeight="1">
+    <row r="50" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -8954,7 +8954,7 @@
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
     </row>
-    <row r="51" spans="1:28" ht="14.1" customHeight="1">
+    <row r="51" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -8998,7 +8998,7 @@
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
     </row>
-    <row r="52" spans="1:28" ht="14.1" customHeight="1">
+    <row r="52" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>50</v>
       </c>

</xml_diff>